<commit_message>
improved the fake data for testing, adding some print statements and comments to notebook, still can not sort colour-coding out
</commit_message>
<xml_diff>
--- a/data/citation_data_fake_prep.xlsx
+++ b/data/citation_data_fake_prep.xlsx
@@ -5,22 +5,57 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nch169_newcastle_ac_uk/Documents/work/sonification_research/sonic_intangibles/si_citationAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nch169_newcastle_ac_uk/Documents/work/sonification_research/sonic_intangibles/si_citationAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{C19A9AE5-DBE8-084F-A686-68B67D5EFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C88DFF29-86CA-E84F-B126-614955D807E9}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{C19A9AE5-DBE8-084F-A686-68B67D5EFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1281B8D-623B-0242-ACBA-718477F7FF14}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="-17640" windowWidth="27640" windowHeight="16680" xr2:uid="{9909D332-0698-EE43-B568-BE5B72009470}"/>
+    <workbookView xWindow="8960" yWindow="5760" windowWidth="27640" windowHeight="16680" xr2:uid="{9909D332-0698-EE43-B568-BE5B72009470}"/>
   </bookViews>
   <sheets>
     <sheet name="citation_data_fake_prep" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="35">
   <si>
     <t>source</t>
   </si>
@@ -643,18 +678,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1030,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CF3F2A-E2F6-9349-97EA-77FF781B373F}">
-  <dimension ref="A1:N154"/>
+  <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,14 +1076,14 @@
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1058,115 +1092,130 @@
       <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q1" t="str" cm="1">
+        <f t="array" ref="Q1:Q27">_xlfn.UNIQUE(B2:B19999)</f>
+        <v>WOS:000279731700009</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q2" t="str">
+        <v>WOS:000396401600013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="I3" s="4"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q3" t="str">
+        <v>WOS:000365063100009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q4" t="str">
+        <v>WOS:001265701800001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="7"/>
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q5" t="str">
+        <v>WOS:000587608600026</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q6" t="str">
+        <v>WOS:000492417900009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q7" t="str">
+        <v>WOS:000380450900007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="7" t="s">
         <v>32</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -1175,178 +1224,200 @@
       <c r="L8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q8" t="str">
+        <v>WOS:001336892600004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q9" t="str">
+        <v>WOS:000279731700007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="L10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q10" t="str">
+        <v>WOS:000274369800014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q11" t="str">
+        <v>WOS:001381043200001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q12" t="str">
+        <v>WOS:000380410400105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q13" t="str">
+        <v>WOS:001087472600001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q14" t="str">
+        <v>WOS:000310847300019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="7"/>
+      <c r="J15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q15" t="str">
+        <v>WOS:001259864900041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5" t="s">
+      <c r="I16" s="7"/>
+      <c r="J16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q16" t="str">
+        <v>WOS:001337593100008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5" t="s">
+      <c r="I17" s="7"/>
+      <c r="J17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q17" t="str">
+        <v>WOS:000484590300001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5" t="s">
+      <c r="I18" s="7"/>
+      <c r="J18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q18" t="str">
+        <v>WOS:001352180500100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="J19" t="s">
@@ -1355,64 +1426,72 @@
       <c r="L19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q19" t="str">
+        <v>WOS:000519098200104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="7"/>
       <c r="J20" t="s">
         <v>21</v>
       </c>
       <c r="L20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q20" t="str">
+        <v>WOS:001337581700004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="I21" s="4"/>
+      <c r="I21" s="7"/>
       <c r="J21" t="s">
         <v>22</v>
       </c>
       <c r="L21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q21" t="str">
+        <v>WOS:000278584300025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="I22" s="4"/>
+      <c r="I22" s="7"/>
       <c r="J22" t="s">
         <v>23</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q22" t="str">
+        <v>WOS:000243205900006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J23" s="2" t="s">
@@ -1421,405 +1500,387 @@
       <c r="L23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q23" t="str">
+        <v>WOS:000345168400011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="I24" s="4"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q24" t="str">
+        <v>WOS:001062040400001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q25" t="str">
+        <v>WOS:000674894000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="L26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q26" t="str">
+        <v>WOS:000573482500002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="7"/>
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="6">
         <f xml:space="preserve"> COUNTIF(L2:L26,"*")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="7"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
         <v>9</v>
       </c>
-      <c r="B60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" t="s">
         <v>10</v>
-      </c>
-      <c r="B65" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1827,7 +1888,7 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1835,7 +1896,7 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1843,23 +1904,23 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1867,15 +1928,15 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B72" t="s">
-        <v>10</v>
+      <c r="B72" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1883,31 +1944,31 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>2</v>
+      <c r="B74" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1915,7 +1976,7 @@
         <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1923,7 +1984,7 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1931,23 +1992,23 @@
         <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1955,7 +2016,7 @@
         <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1963,7 +2024,7 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1971,23 +2032,23 @@
         <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>14</v>
+      <c r="A85" t="s">
+        <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>14</v>
+      <c r="A86" t="s">
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,7 +2056,7 @@
         <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -2003,23 +2064,23 @@
         <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
         <v>15</v>
-      </c>
-      <c r="B89" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -2027,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -2035,23 +2096,23 @@
         <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
         <v>16</v>
-      </c>
-      <c r="B94" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -2059,7 +2120,7 @@
         <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -2067,23 +2128,23 @@
         <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -2091,7 +2152,7 @@
         <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -2099,7 +2160,7 @@
         <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -2107,23 +2168,23 @@
         <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -2131,7 +2192,7 @@
         <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -2139,23 +2200,23 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B107" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -2163,7 +2224,7 @@
         <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -2171,7 +2232,7 @@
         <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -2179,23 +2240,23 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
         <v>20</v>
-      </c>
-      <c r="B112" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -2203,7 +2264,7 @@
         <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2211,23 +2272,23 @@
         <v>21</v>
       </c>
       <c r="B114" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B115" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>22</v>
+      </c>
+      <c r="B116" t="s">
         <v>21</v>
-      </c>
-      <c r="B116" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -2235,7 +2296,7 @@
         <v>22</v>
       </c>
       <c r="B117" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -2243,23 +2304,23 @@
         <v>22</v>
       </c>
       <c r="B118" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B119" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -2267,7 +2328,7 @@
         <v>23</v>
       </c>
       <c r="B121" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -2275,23 +2336,23 @@
         <v>23</v>
       </c>
       <c r="B122" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B124" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -2299,7 +2360,7 @@
         <v>24</v>
       </c>
       <c r="B125" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -2307,23 +2368,23 @@
         <v>24</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>25</v>
+      </c>
+      <c r="B128" t="s">
         <v>24</v>
-      </c>
-      <c r="B128" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -2331,7 +2392,7 @@
         <v>25</v>
       </c>
       <c r="B129" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -2339,23 +2400,23 @@
         <v>25</v>
       </c>
       <c r="B130" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B131" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B132" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -2363,7 +2424,7 @@
         <v>26</v>
       </c>
       <c r="B133" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -2371,7 +2432,7 @@
         <v>26</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -2379,23 +2440,23 @@
         <v>26</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B137" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -2403,7 +2464,7 @@
         <v>27</v>
       </c>
       <c r="B138" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -2411,7 +2472,7 @@
         <v>27</v>
       </c>
       <c r="B139" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -2419,15 +2480,15 @@
         <v>27</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -2435,7 +2496,7 @@
         <v>26</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -2443,15 +2504,15 @@
         <v>26</v>
       </c>
       <c r="B143" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B144" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -2459,7 +2520,7 @@
         <v>27</v>
       </c>
       <c r="B145" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -2467,7 +2528,7 @@
         <v>27</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -2475,15 +2536,15 @@
         <v>27</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B148" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -2491,15 +2552,15 @@
         <v>26</v>
       </c>
       <c r="B149" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B150" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
@@ -2507,7 +2568,7 @@
         <v>27</v>
       </c>
       <c r="B151" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -2515,7 +2576,7 @@
         <v>27</v>
       </c>
       <c r="B152" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -2523,14 +2584,6 @@
         <v>27</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>27</v>
-      </c>
-      <c r="B154" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>